<commit_message>
Finished the main program. Just need to figure out how to publish it.
</commit_message>
<xml_diff>
--- a/Result/Result3.xlsx
+++ b/Result/Result3.xlsx
@@ -5,15 +5,53 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Architectural Technology and Co" sheetId="1" r:id="rId1"/>
-    <sheet name="Automation Engineering.xlsx" sheetId="2" r:id="rId3"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Architectural Technology and Co" sheetId="2" r:id="rId3"/>
+    <sheet name="Automation Engineering.xlsx" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <si>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:sz val="24"/>
+        <d:rFont val="Calibri"/>
+      </d:rPr>
+      <d:t xml:space="preserve">General Overview</d:t>
+    </d:r>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Total Students</t>
+  </si>
+  <si>
+    <t>Students in DK</t>
+  </si>
+  <si>
+    <t>% of Students in DK</t>
+  </si>
+  <si>
+    <t>Architectural Technology and Construction Management.xlsx</t>
+  </si>
+  <si>
+    <t>Automation Engineering.xlsx</t>
+  </si>
+  <si>
+    <t>All Students</t>
+  </si>
+  <si>
+    <t>All Students in DK</t>
+  </si>
+  <si>
+    <t>% of All Students in DK</t>
+  </si>
   <si>
     <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <d:rPr>
@@ -163,7 +201,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +218,23 @@
         <fgColor rgb="FFD3D3D3" tint="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF98FB98" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDB7093" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFEEEE" tint="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,14 +242,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="4" applyFill="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="5" applyFill="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="0" applyFont="1" fillId="6" applyFill="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -207,7 +287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -219,178 +299,324 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="0">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B5" s="0">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="0" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="0" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="0" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="0" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="0" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="0" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="0" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="0" t="b">
-        <v>1</v>
+      <c r="A8" s="0">
+        <f>=SUM(B4:B5)</f>
+      </c>
+      <c r="B8" s="0">
+        <f>=SUM(C4:C5)</f>
+      </c>
+      <c r="C8" s="0">
+        <f>=(B8/A8)</f>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.722591400146484" customWidth="1"/>
+    <col min="2" max="2" width="16.837453842163086" customWidth="1"/>
+    <col min="3" max="3" width="23.259233474731445" customWidth="1"/>
+    <col min="4" max="4" width="12.424972534179688" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8">
+        <f>=(C4/B4)</f>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>8</v>
+      </c>
+      <c r="B14" s="0">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8">
+        <f>=(B14/A14)</f>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.098708152770996" customWidth="1"/>
+    <col min="2" max="2" width="16.837453842163086" customWidth="1"/>
+    <col min="3" max="3" width="18.66567039489746" customWidth="1"/>
+    <col min="4" max="4" width="12.424972534179688" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="0" t="b">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="D4" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="8">
+        <f>=(C5/B5)</f>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>1</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <f>=(B7/A7)</f>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>